<commit_message>
modified:   data_sheets/Sensor_Power_Model.xlsx 	modified:   data_sheets/Simple_Power_Model.pdf
</commit_message>
<xml_diff>
--- a/data_sheets/Sensor_Power_Model.xlsx
+++ b/data_sheets/Sensor_Power_Model.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uwnetid-my.sharepoint.com/personal/jingyj11_uw_edu/Documents/2024winter/514 SWHWLab/Hydration Companion/data_sheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="8_{4E7FDCB4-83D0-40CF-AFF0-2E9F2538FC30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9A179A6E-B3D3-4905-B7E0-9A40C3201D96}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="8_{4E7FDCB4-83D0-40CF-AFF0-2E9F2538FC30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{81FA80C9-6A4A-47CD-BD54-C3F5FD7FA389}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -198,12 +198,6 @@
     <t>500K</t>
   </si>
   <si>
-    <t>https://github.com/Jingyii800/Hydration-Companion/blob/main/data_sheets/SSD1306.pdf</t>
-  </si>
-  <si>
-    <t>https://github.com/Jingyii800/Hydration-Companion/blob/main/data_sheets/Stepper-motor2424.pdf</t>
-  </si>
-  <si>
     <t>https://github.com/Jingyii800/Hydration-Companion/blob/main/data_sheets/1498852.pdf</t>
   </si>
   <si>
@@ -214,6 +208,12 @@
   </si>
   <si>
     <t>Buzzer</t>
+  </si>
+  <si>
+    <t>https://github.com/Jingyii800/Hydration-Companion/blob/main/data_sheets/ef532_ps-13444.pdf</t>
+  </si>
+  <si>
+    <t>https://github.com/Jingyii800/Hydration-Companion/blob/main/data_sheets/hx71_english.pdf</t>
   </si>
 </sst>
 </file>
@@ -1585,7 +1585,7 @@
   <dimension ref="A1:R45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1596,7 +1596,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="23" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1720,7 +1720,7 @@
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="I11" s="6"/>
     </row>
@@ -1755,10 +1755,10 @@
     </row>
     <row r="15" spans="1:9" ht="13" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B15" s="26" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="I15" s="6"/>
     </row>
@@ -1831,10 +1831,10 @@
     </row>
     <row r="20" spans="1:17" ht="13" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B20" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="I20" s="6"/>
     </row>
@@ -2319,12 +2319,9 @@
       <c r="R45" s="27"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B15" r:id="rId1" xr:uid="{2BE6C8CC-E46B-4AE7-9BBC-C5173E9790ED}"/>
-  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="66" orientation="landscape" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
-  <drawing r:id="rId3"/>
+  <pageSetup paperSize="66" orientation="landscape" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -3111,7 +3108,7 @@
       </c>
       <c r="B64" s="9" t="str">
         <f>'System Parameters'!B15</f>
-        <v>https://github.com/Jingyii800/Hydration-Companion/blob/main/data_sheets/Stepper-motor2424.pdf</v>
+        <v>https://github.com/Jingyii800/Hydration-Companion/blob/main/data_sheets/hx71_english.pdf</v>
       </c>
       <c r="C64" s="9">
         <f>'System Parameters'!C15</f>
@@ -3119,51 +3116,51 @@
       </c>
       <c r="D64" s="9" t="str">
         <f t="shared" si="1"/>
-        <v>https://github.com/Jingyii800/Hydration-Companion/blob/main/data_sheets/Stepper-motor2424.pdf</v>
+        <v>https://github.com/Jingyii800/Hydration-Companion/blob/main/data_sheets/hx71_english.pdf</v>
       </c>
       <c r="E64" s="9" t="str">
         <f t="shared" si="3"/>
-        <v>https://github.com/Jingyii800/Hydration-Companion/blob/main/data_sheets/Stepper-motor2424.pdf</v>
+        <v>https://github.com/Jingyii800/Hydration-Companion/blob/main/data_sheets/hx71_english.pdf</v>
       </c>
       <c r="F64" s="9" t="str">
         <f t="shared" si="5"/>
-        <v>https://github.com/Jingyii800/Hydration-Companion/blob/main/data_sheets/Stepper-motor2424.pdf</v>
+        <v>https://github.com/Jingyii800/Hydration-Companion/blob/main/data_sheets/hx71_english.pdf</v>
       </c>
       <c r="G64" s="9" t="str">
         <f t="shared" si="7"/>
-        <v>https://github.com/Jingyii800/Hydration-Companion/blob/main/data_sheets/Stepper-motor2424.pdf</v>
+        <v>https://github.com/Jingyii800/Hydration-Companion/blob/main/data_sheets/hx71_english.pdf</v>
       </c>
       <c r="H64" s="9" t="str">
         <f t="shared" si="6"/>
-        <v>https://github.com/Jingyii800/Hydration-Companion/blob/main/data_sheets/Stepper-motor2424.pdf</v>
+        <v>https://github.com/Jingyii800/Hydration-Companion/blob/main/data_sheets/hx71_english.pdf</v>
       </c>
       <c r="I64" s="9" t="str">
         <f t="shared" si="6"/>
-        <v>https://github.com/Jingyii800/Hydration-Companion/blob/main/data_sheets/Stepper-motor2424.pdf</v>
+        <v>https://github.com/Jingyii800/Hydration-Companion/blob/main/data_sheets/hx71_english.pdf</v>
       </c>
       <c r="J64" s="9" t="str">
         <f t="shared" si="6"/>
-        <v>https://github.com/Jingyii800/Hydration-Companion/blob/main/data_sheets/Stepper-motor2424.pdf</v>
+        <v>https://github.com/Jingyii800/Hydration-Companion/blob/main/data_sheets/hx71_english.pdf</v>
       </c>
       <c r="K64" s="9" t="str">
         <f t="shared" si="6"/>
-        <v>https://github.com/Jingyii800/Hydration-Companion/blob/main/data_sheets/Stepper-motor2424.pdf</v>
+        <v>https://github.com/Jingyii800/Hydration-Companion/blob/main/data_sheets/hx71_english.pdf</v>
       </c>
       <c r="L64" s="9" t="str">
         <f t="shared" si="6"/>
-        <v>https://github.com/Jingyii800/Hydration-Companion/blob/main/data_sheets/Stepper-motor2424.pdf</v>
+        <v>https://github.com/Jingyii800/Hydration-Companion/blob/main/data_sheets/hx71_english.pdf</v>
       </c>
       <c r="M64" s="9" t="str">
         <f t="shared" si="6"/>
-        <v>https://github.com/Jingyii800/Hydration-Companion/blob/main/data_sheets/Stepper-motor2424.pdf</v>
+        <v>https://github.com/Jingyii800/Hydration-Companion/blob/main/data_sheets/hx71_english.pdf</v>
       </c>
       <c r="N64" s="9" t="str">
         <f t="shared" si="6"/>
-        <v>https://github.com/Jingyii800/Hydration-Companion/blob/main/data_sheets/Stepper-motor2424.pdf</v>
+        <v>https://github.com/Jingyii800/Hydration-Companion/blob/main/data_sheets/hx71_english.pdf</v>
       </c>
       <c r="O64" s="9" t="str">
         <f t="shared" si="6"/>
-        <v>https://github.com/Jingyii800/Hydration-Companion/blob/main/data_sheets/Stepper-motor2424.pdf</v>
+        <v>https://github.com/Jingyii800/Hydration-Companion/blob/main/data_sheets/hx71_english.pdf</v>
       </c>
       <c r="T64" s="9">
         <f>'System Parameters'!E15</f>
@@ -3501,7 +3498,7 @@
       </c>
       <c r="B69" s="9" t="str">
         <f>'System Parameters'!B20</f>
-        <v>https://github.com/Jingyii800/Hydration-Companion/blob/main/data_sheets/SSD1306.pdf</v>
+        <v>https://github.com/Jingyii800/Hydration-Companion/blob/main/data_sheets/ef532_ps-13444.pdf</v>
       </c>
       <c r="C69" s="9">
         <f>'System Parameters'!C20</f>
@@ -3509,51 +3506,51 @@
       </c>
       <c r="D69" s="9" t="str">
         <f t="shared" si="1"/>
-        <v>https://github.com/Jingyii800/Hydration-Companion/blob/main/data_sheets/SSD1306.pdf</v>
+        <v>https://github.com/Jingyii800/Hydration-Companion/blob/main/data_sheets/ef532_ps-13444.pdf</v>
       </c>
       <c r="E69" s="9" t="str">
         <f t="shared" si="3"/>
-        <v>https://github.com/Jingyii800/Hydration-Companion/blob/main/data_sheets/SSD1306.pdf</v>
+        <v>https://github.com/Jingyii800/Hydration-Companion/blob/main/data_sheets/ef532_ps-13444.pdf</v>
       </c>
       <c r="F69" s="9" t="str">
         <f t="shared" si="5"/>
-        <v>https://github.com/Jingyii800/Hydration-Companion/blob/main/data_sheets/SSD1306.pdf</v>
+        <v>https://github.com/Jingyii800/Hydration-Companion/blob/main/data_sheets/ef532_ps-13444.pdf</v>
       </c>
       <c r="G69" s="9" t="str">
         <f t="shared" si="7"/>
-        <v>https://github.com/Jingyii800/Hydration-Companion/blob/main/data_sheets/SSD1306.pdf</v>
+        <v>https://github.com/Jingyii800/Hydration-Companion/blob/main/data_sheets/ef532_ps-13444.pdf</v>
       </c>
       <c r="H69" s="9" t="str">
         <f t="shared" si="9"/>
-        <v>https://github.com/Jingyii800/Hydration-Companion/blob/main/data_sheets/SSD1306.pdf</v>
+        <v>https://github.com/Jingyii800/Hydration-Companion/blob/main/data_sheets/ef532_ps-13444.pdf</v>
       </c>
       <c r="I69" s="9" t="str">
         <f t="shared" si="11"/>
-        <v>https://github.com/Jingyii800/Hydration-Companion/blob/main/data_sheets/SSD1306.pdf</v>
+        <v>https://github.com/Jingyii800/Hydration-Companion/blob/main/data_sheets/ef532_ps-13444.pdf</v>
       </c>
       <c r="J69" s="9" t="str">
         <f t="shared" si="13"/>
-        <v>https://github.com/Jingyii800/Hydration-Companion/blob/main/data_sheets/SSD1306.pdf</v>
+        <v>https://github.com/Jingyii800/Hydration-Companion/blob/main/data_sheets/ef532_ps-13444.pdf</v>
       </c>
       <c r="K69" s="9" t="str">
         <f t="shared" si="12"/>
-        <v>https://github.com/Jingyii800/Hydration-Companion/blob/main/data_sheets/SSD1306.pdf</v>
+        <v>https://github.com/Jingyii800/Hydration-Companion/blob/main/data_sheets/ef532_ps-13444.pdf</v>
       </c>
       <c r="L69" s="9" t="str">
         <f t="shared" si="12"/>
-        <v>https://github.com/Jingyii800/Hydration-Companion/blob/main/data_sheets/SSD1306.pdf</v>
+        <v>https://github.com/Jingyii800/Hydration-Companion/blob/main/data_sheets/ef532_ps-13444.pdf</v>
       </c>
       <c r="M69" s="9" t="str">
         <f t="shared" si="12"/>
-        <v>https://github.com/Jingyii800/Hydration-Companion/blob/main/data_sheets/SSD1306.pdf</v>
+        <v>https://github.com/Jingyii800/Hydration-Companion/blob/main/data_sheets/ef532_ps-13444.pdf</v>
       </c>
       <c r="N69" s="9" t="str">
         <f t="shared" si="12"/>
-        <v>https://github.com/Jingyii800/Hydration-Companion/blob/main/data_sheets/SSD1306.pdf</v>
+        <v>https://github.com/Jingyii800/Hydration-Companion/blob/main/data_sheets/ef532_ps-13444.pdf</v>
       </c>
       <c r="O69" s="9" t="str">
         <f t="shared" si="12"/>
-        <v>https://github.com/Jingyii800/Hydration-Companion/blob/main/data_sheets/SSD1306.pdf</v>
+        <v>https://github.com/Jingyii800/Hydration-Companion/blob/main/data_sheets/ef532_ps-13444.pdf</v>
       </c>
       <c r="T69" s="9">
         <f>'System Parameters'!E20</f>

</xml_diff>